<commit_message>
FW: PHTS + ISR notes
</commit_message>
<xml_diff>
--- a/DOCS/Notes/phts_sensor_calc_example.xlsx
+++ b/DOCS/Notes/phts_sensor_calc_example.xlsx
@@ -18,30 +18,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
-    <t>c1</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>c3</t>
-  </si>
-  <si>
-    <t>c4</t>
-  </si>
-  <si>
-    <t>c5</t>
-  </si>
-  <si>
-    <t>c6</t>
-  </si>
-  <si>
     <t>dT</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
     <t>Temp</t>
   </si>
   <si>
@@ -135,9 +114,6 @@
     <t>pt_coef_t{data}@0x0124</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>Off</t>
   </si>
   <si>
@@ -160,6 +136,31 @@
   </si>
   <si>
     <t>P = D1 * SENS - OFF = (D1 * SENS / 2^21 - OFF) / 2^15</t>
+  </si>
+  <si>
+    <t>D2 (adcT)</t>
+  </si>
+  <si>
+    <t>D1 (adcP)</t>
+  </si>
+  <si>
+    <t>1.dT</t>
+  </si>
+  <si>
+    <t>2.off</t>
+  </si>
+  <si>
+    <t>3.sens</t>
+  </si>
+  <si>
+    <t>4.p</t>
+  </si>
+  <si>
+    <t>5.t</t>
+  </si>
+  <si>
+    <t>dT = D2 - TREF = D2 - C5 * 2^8       (24bit)
+TEMP = 20°C + dT *TEMPSENS = 2000 + dT * C6 / 2^23</t>
   </si>
 </sst>
 </file>
@@ -195,8 +196,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,406 +502,523 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A6:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" customWidth="1"/>
+    <col min="7" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>29125</v>
-      </c>
-      <c r="D5" t="str">
-        <f>DEC2HEX(C5)</f>
-        <v>71C5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>28165</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" ref="D6:D9" si="0">DEC2HEX(C6)</f>
-        <v>6E05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6">
+        <f>($B$9 - G31)</f>
+        <v>437</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <f>G6 * G30 / 2^15</f>
+        <v>341.21954345703125</v>
+      </c>
+      <c r="H7">
+        <f>FLOOR(G6*G30*4,1)</f>
+        <v>44724328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B8">
-        <v>25286</v>
+        <v>25449</v>
       </c>
       <c r="C8">
         <f>B8*256</f>
-        <v>6473216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6514944</v>
+      </c>
+      <c r="G8">
+        <f>G28+G7</f>
+        <v>42287.219543457031</v>
+      </c>
+      <c r="H8">
+        <f>H7+G28*2^17</f>
+        <v>5542670440</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B9">
-        <v>29750</v>
+        <v>29562</v>
       </c>
       <c r="C9">
         <f>B9*256</f>
-        <v>7616000</v>
+        <v>7567872</v>
       </c>
       <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>743600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D6:D9" si="0">DEC2HEX(C9)</f>
+        <v>737A00</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <f>G6*G29/2^15</f>
+        <v>387.74948120117187</v>
+      </c>
+      <c r="H9">
+        <f>G6*G29*2</f>
+        <v>25411550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>(G9+G27)</f>
+        <v>43680.749481201172</v>
+      </c>
+      <c r="H10">
+        <f>H9+G27*2^16</f>
+        <v>2862661598</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f>C9-C5*256</f>
-        <v>160000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <f>C9-G31*256</f>
+        <v>111872</v>
+      </c>
+      <c r="D11">
+        <f>C11/256</f>
+        <v>437</v>
+      </c>
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <f>($B$8 * G10)/2^15</f>
+        <v>33924.297898775898</v>
+      </c>
+      <c r="H11">
+        <f>B8*H10/2^13</f>
+        <v>8893051148.376709</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <f>C11*C6/2^23</f>
-        <v>537.20474243164063</v>
+        <f>C11*G32/2^23</f>
+        <v>356.24942016601562</v>
       </c>
       <c r="D12">
         <f t="shared" ref="D12" si="1">D11*D6/2^23</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f>(2*G11-G8)</f>
+        <v>25561.376254094765</v>
+      </c>
+      <c r="H12">
+        <f>H11-H8</f>
+        <v>3350380708.376709</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <f>2000+C12</f>
-        <v>2537.2047424316406</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15">
-        <f>G24*2^17 + G26/2^6</f>
-        <v>5497946511.78125</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2356.2494201660156</v>
+      </c>
+      <c r="G13">
+        <f>G12*2^2</f>
+        <v>102245.50501637906</v>
+      </c>
+      <c r="H13">
+        <f>FLOOR(H12/2^15,1)</f>
+        <v>102245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15">
+        <f>G6*G32/2^17</f>
+        <v>89.062355041503906</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <f>G28*2^17 + G30*C11/2^6</f>
+        <v>5542670440</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <f>B16/256</f>
+        <v>21651056.40625</v>
+      </c>
+      <c r="G16">
+        <f>2000+G6*G32/2^15</f>
+        <v>2356.2494201660156</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="B17">
+        <f>G30*C11/2^6</f>
+        <v>44724328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>33</v>
-      </c>
-      <c r="G17">
-        <v>6465635</v>
-      </c>
-      <c r="H17" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19">
-        <f>G23*2^16+G25*C11/2^7</f>
-        <v>2873593798</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" t="s">
-        <v>11</v>
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19">
+        <v>6465635</v>
+      </c>
+      <c r="I19" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B21">
-        <f>(C8*B19/2^21 - B15)/2^15</f>
-        <v>102901.88696874678</v>
-      </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>36</v>
-      </c>
-      <c r="G21" t="s">
+        <f>G27*2^16+G29*C11/2^7</f>
+        <v>2862661598</v>
+      </c>
+      <c r="E21">
+        <f>B21/256</f>
+        <v>11182271.8671875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f>G29*C11/2^7</f>
+        <v>25411550</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="H21" t="s">
+      <c r="P24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="O21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22">
+      <c r="B25">
+        <f>(C8*B21/2^21 - B16)/2^15</f>
+        <v>102245.50501637906</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" t="s">
+        <v>31</v>
+      </c>
+      <c r="P25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <f>C8*B21/2^21</f>
+        <v>8893051148.376709</v>
+      </c>
+      <c r="F26" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26">
         <v>2977</v>
       </c>
-      <c r="H22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" t="str">
-        <f>DEC2HEX(G22)</f>
+      <c r="H26">
+        <v>2977</v>
+      </c>
+      <c r="I26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" t="str">
+        <f>DEC2HEX(G26)</f>
         <v>BA1</v>
       </c>
-      <c r="O22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23">
+      <c r="P26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <f>(C8*B21/2^21 - B16)</f>
+        <v>3350380708.376709</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27">
         <v>43293</v>
       </c>
-      <c r="H23" t="s">
-        <v>13</v>
-      </c>
-      <c r="I23" t="str">
-        <f t="shared" ref="I23:I28" si="2">DEC2HEX(G23)</f>
+      <c r="H27">
+        <v>43293</v>
+      </c>
+      <c r="I27" t="s">
+        <v>6</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" ref="J27:J32" si="2">DEC2HEX(G27)</f>
         <v>A91D</v>
       </c>
-      <c r="O23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F24" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24">
+      <c r="P27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <f>B27/2^15</f>
+        <v>102245.50501637906</v>
+      </c>
+      <c r="F28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28">
         <v>41946</v>
       </c>
-      <c r="H24" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" t="str">
+      <c r="H28">
+        <v>41946</v>
+      </c>
+      <c r="I28" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" t="str">
         <f t="shared" si="2"/>
         <v>A3DA</v>
       </c>
-      <c r="O24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25">
+      <c r="P28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29">
         <v>29075</v>
       </c>
-      <c r="H25" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" t="str">
+      <c r="H29">
+        <f>29075/2^15</f>
+        <v>0.887298583984375</v>
+      </c>
+      <c r="I29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" t="str">
         <f t="shared" si="2"/>
         <v>7193</v>
       </c>
-      <c r="O25" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26">
+      <c r="P29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30">
         <v>25586</v>
       </c>
-      <c r="H26" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" t="str">
+      <c r="H30">
+        <f>25586/2^15</f>
+        <v>0.78082275390625</v>
+      </c>
+      <c r="I30" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30" t="str">
         <f t="shared" si="2"/>
         <v>63F2</v>
       </c>
-      <c r="O26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27">
+      <c r="P30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31">
         <v>29125</v>
       </c>
-      <c r="H27" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" t="str">
+      <c r="H31">
+        <v>29125</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" t="str">
         <f t="shared" si="2"/>
         <v>71C5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f xml:space="preserve"> G30*C11/2^6</f>
+        <v>44724328</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32">
         <v>26713</v>
       </c>
-      <c r="H28" t="s">
-        <v>23</v>
-      </c>
-      <c r="I28" t="str">
+      <c r="H32">
+        <v>26713</v>
+      </c>
+      <c r="I32" t="s">
+        <v>16</v>
+      </c>
+      <c r="J32" t="str">
         <f t="shared" si="2"/>
         <v>6859</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N32" t="s">
+    <row r="36" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>3</v>
+      </c>
+      <c r="P36">
+        <v>48033</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P37">
+        <v>43293</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O38" t="s">
+        <v>7</v>
+      </c>
+      <c r="P38">
+        <v>41946</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
+        <v>9</v>
+      </c>
+      <c r="P39">
+        <v>29075</v>
+      </c>
+      <c r="Q39" t="s">
         <v>10</v>
       </c>
-      <c r="O32">
-        <v>48033</v>
-      </c>
-      <c r="P32" t="s">
+    </row>
+    <row r="40" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N33" t="s">
+      <c r="P40">
+        <v>25586</v>
+      </c>
+      <c r="Q40" t="s">
         <v>12</v>
       </c>
-      <c r="O33">
-        <v>43293</v>
-      </c>
-      <c r="P33" t="s">
+    </row>
+    <row r="41" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N34" t="s">
+      <c r="P41">
+        <v>29125</v>
+      </c>
+      <c r="Q41" t="s">
         <v>14</v>
       </c>
-      <c r="O34">
-        <v>41946</v>
-      </c>
-      <c r="P34" t="s">
+    </row>
+    <row r="42" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O42" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N35" t="s">
+      <c r="P42">
+        <v>26713</v>
+      </c>
+      <c r="Q42" t="s">
         <v>16</v>
       </c>
-      <c r="O35">
-        <v>29075</v>
-      </c>
-      <c r="P35" t="s">
+    </row>
+    <row r="43" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O43" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N36" t="s">
+      <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="s">
         <v>18</v>
-      </c>
-      <c r="O36">
-        <v>25586</v>
-      </c>
-      <c r="P36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N37" t="s">
-        <v>20</v>
-      </c>
-      <c r="O37">
-        <v>29125</v>
-      </c>
-      <c r="P37" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N38" t="s">
-        <v>22</v>
-      </c>
-      <c r="O38">
-        <v>26713</v>
-      </c>
-      <c r="P38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N39" t="s">
-        <v>24</v>
-      </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-      <c r="P39" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>